<commit_message>
melting data to fit metafor analysis structure in new file, averaging treatments that did not share the same mean as flux, saving dated version of full dataset
</commit_message>
<xml_diff>
--- a/data extraction /extraction /raw data /duncan2016/duncan2016.xlsx
+++ b/data extraction /extraction /raw data /duncan2016/duncan2016.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /raw data /duncan2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB68DEFC-ECB8-5441-A745-67779E604299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80573D8F-8EEC-FF4E-8313-38E1A17D81BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15120" activeTab="1" xr2:uid="{B950434C-E0CC-7B40-865F-77A247B1A484}"/>
+    <workbookView xWindow="1180" yWindow="1240" windowWidth="27240" windowHeight="15120" activeTab="1" xr2:uid="{B950434C-E0CC-7B40-865F-77A247B1A484}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
     <sheet name="cleaned" sheetId="2" r:id="rId2"/>
+    <sheet name="metafor calcs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
   <si>
     <t>x</t>
   </si>
@@ -65,6 +66,12 @@
   </si>
   <si>
     <t>32/32</t>
+  </si>
+  <si>
+    <t>avg_constant</t>
+  </si>
+  <si>
+    <t>avg_constant_error</t>
   </si>
 </sst>
 </file>
@@ -80,12 +87,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,10 +789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16709E1-323A-3340-BA53-02FC4A15E9DA}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="B9" sqref="B9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,7 +863,37 @@
         <v>0.11413026183595801</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <f>AVERAGE(A2,A4)</f>
+        <v>-2.3909825023451015E-2</v>
+      </c>
+      <c r="C10" s="1">
+        <f>AVERAGE(C2,C4)</f>
+        <v>0.11820634261581375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F339634-1AAB-3F46-9FAF-1803C58F3370}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>